<commit_message>
adding area to all discharge files
</commit_message>
<xml_diff>
--- a/Discharge/Station2_2021-07-20_1308.xlsx
+++ b/Discharge/Station2_2021-07-20_1308.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{8D2C956D-2AC7-4AD5-B1C6-DD3276D58094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68F39CD7-D19D-49FE-837F-7467ED7DEA94}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="340" windowWidth="14290" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9090" yWindow="1000" windowWidth="10110" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,6 +110,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>